<commit_message>
Changes made to project plan and proposal
- Completed project plan for 19 weeks.
- Added proposed programming language section to the proposal
</commit_message>
<xml_diff>
--- a/FYP_Project_Plan.xlsx
+++ b/FYP_Project_Plan.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>PERIODS</t>
   </si>
@@ -191,7 +191,16 @@
     <t xml:space="preserve">Elaboration </t>
   </si>
   <si>
-    <t>Full Project</t>
+    <t>Construction 1 : Building App</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cunstruction 2 : Testing </t>
+  </si>
+  <si>
+    <t>Full projrct time line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transition </t>
   </si>
 </sst>
 </file>
@@ -564,6 +573,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -576,15 +591,21 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -608,18 +629,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1030,10 +1039,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO30"/>
+  <dimension ref="B1:GD30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="65" zoomScaleNormal="65" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="59" zoomScaleNormal="59" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1042,11 +1051,12 @@
     <col min="2" max="2" width="36.6640625" style="2" customWidth="1"/>
     <col min="3" max="6" width="11.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" style="4" customWidth="1"/>
-    <col min="8" max="27" width="2.77734375" style="1"/>
+    <col min="8" max="8" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="27" width="2.77734375" style="1"/>
     <col min="34" max="34" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="1" spans="2:186" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
       <c r="B1" s="13" t="s">
         <v>22</v>
       </c>
@@ -1056,81 +1066,81 @@
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
     </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+    <row r="2" spans="2:186" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="14">
+        <v>12</v>
+      </c>
+      <c r="J2" s="15"/>
+      <c r="K2" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="19"/>
+      <c r="AI2" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="24"/>
+      <c r="AK2" s="24"/>
+      <c r="AL2" s="24"/>
+      <c r="AM2" s="24"/>
+      <c r="AN2" s="24"/>
+      <c r="AO2" s="24"/>
+      <c r="AP2" s="24"/>
+    </row>
+    <row r="3" spans="2:186" s="11" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
-      <c r="AF2" s="34"/>
-      <c r="AG2" s="35"/>
-      <c r="AH2" s="19"/>
-      <c r="AI2" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ2" s="22"/>
-      <c r="AK2" s="22"/>
-      <c r="AL2" s="22"/>
-      <c r="AM2" s="22"/>
-      <c r="AN2" s="22"/>
-      <c r="AO2" s="22"/>
-      <c r="AP2" s="22"/>
-    </row>
-    <row r="3" spans="2:67" s="11" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="30" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="20" t="s">
@@ -1156,13 +1166,13 @@
       <c r="Z3" s="10"/>
       <c r="AA3" s="10"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="26"/>
+    <row r="4" spans="2:186" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="27"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="31"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1343,240 +1353,631 @@
       <c r="BO4" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="38" t="s">
+      <c r="BP4" s="3">
+        <v>61</v>
+      </c>
+      <c r="BQ4" s="3">
+        <v>62</v>
+      </c>
+      <c r="BR4" s="3">
+        <v>63</v>
+      </c>
+      <c r="BS4" s="3">
+        <v>64</v>
+      </c>
+      <c r="BT4" s="3">
+        <v>65</v>
+      </c>
+      <c r="BU4" s="3">
+        <v>66</v>
+      </c>
+      <c r="BV4" s="3">
+        <v>67</v>
+      </c>
+      <c r="BW4" s="3">
+        <v>68</v>
+      </c>
+      <c r="BX4" s="3">
+        <v>69</v>
+      </c>
+      <c r="BY4" s="3">
+        <v>70</v>
+      </c>
+      <c r="BZ4" s="3">
+        <v>71</v>
+      </c>
+      <c r="CA4" s="3">
+        <v>72</v>
+      </c>
+      <c r="CB4" s="3">
+        <v>73</v>
+      </c>
+      <c r="CC4" s="3">
+        <v>74</v>
+      </c>
+      <c r="CD4" s="3">
+        <v>75</v>
+      </c>
+      <c r="CE4" s="3">
+        <v>76</v>
+      </c>
+      <c r="CF4" s="3">
+        <v>77</v>
+      </c>
+      <c r="CG4" s="3">
+        <v>78</v>
+      </c>
+      <c r="CH4" s="3">
+        <v>79</v>
+      </c>
+      <c r="CI4" s="3">
+        <v>80</v>
+      </c>
+      <c r="CJ4" s="3">
+        <v>81</v>
+      </c>
+      <c r="CK4" s="3">
+        <v>82</v>
+      </c>
+      <c r="CL4" s="3">
+        <v>83</v>
+      </c>
+      <c r="CM4" s="3">
+        <v>84</v>
+      </c>
+      <c r="CN4" s="3">
+        <v>85</v>
+      </c>
+      <c r="CO4" s="3">
+        <v>86</v>
+      </c>
+      <c r="CP4" s="3">
+        <v>87</v>
+      </c>
+      <c r="CQ4" s="3">
+        <v>88</v>
+      </c>
+      <c r="CR4" s="3">
+        <v>89</v>
+      </c>
+      <c r="CS4" s="3">
+        <v>90</v>
+      </c>
+      <c r="CT4" s="3">
+        <v>91</v>
+      </c>
+      <c r="CU4" s="3">
+        <v>92</v>
+      </c>
+      <c r="CV4" s="3">
+        <v>93</v>
+      </c>
+      <c r="CW4" s="3">
+        <v>94</v>
+      </c>
+      <c r="CX4" s="3">
+        <v>95</v>
+      </c>
+      <c r="CY4" s="3">
+        <v>96</v>
+      </c>
+      <c r="CZ4" s="3">
+        <v>97</v>
+      </c>
+      <c r="DA4" s="3">
+        <v>98</v>
+      </c>
+      <c r="DB4" s="3">
+        <v>99</v>
+      </c>
+      <c r="DC4" s="3">
+        <v>100</v>
+      </c>
+      <c r="DD4" s="3">
+        <v>101</v>
+      </c>
+      <c r="DE4" s="3">
+        <v>102</v>
+      </c>
+      <c r="DF4" s="3">
+        <v>103</v>
+      </c>
+      <c r="DG4" s="3">
+        <v>104</v>
+      </c>
+      <c r="DH4" s="3">
+        <v>105</v>
+      </c>
+      <c r="DI4" s="3">
+        <v>106</v>
+      </c>
+      <c r="DJ4" s="3">
+        <v>107</v>
+      </c>
+      <c r="DK4" s="3">
+        <v>108</v>
+      </c>
+      <c r="DL4" s="3">
+        <v>109</v>
+      </c>
+      <c r="DM4" s="3">
+        <v>110</v>
+      </c>
+      <c r="DN4" s="3">
+        <v>111</v>
+      </c>
+      <c r="DO4" s="3">
+        <v>112</v>
+      </c>
+      <c r="DP4" s="3">
+        <v>113</v>
+      </c>
+      <c r="DQ4" s="3">
+        <v>114</v>
+      </c>
+      <c r="DR4" s="3">
+        <v>115</v>
+      </c>
+      <c r="DS4" s="3">
+        <v>116</v>
+      </c>
+      <c r="DT4" s="3">
+        <v>117</v>
+      </c>
+      <c r="DU4" s="3">
+        <v>118</v>
+      </c>
+      <c r="DV4" s="3">
+        <v>119</v>
+      </c>
+      <c r="DW4" s="3">
+        <v>120</v>
+      </c>
+      <c r="DX4" s="3">
+        <v>121</v>
+      </c>
+      <c r="DY4" s="3">
+        <v>122</v>
+      </c>
+      <c r="DZ4" s="3">
+        <v>123</v>
+      </c>
+      <c r="EA4" s="3">
+        <v>124</v>
+      </c>
+      <c r="EB4" s="3">
+        <v>125</v>
+      </c>
+      <c r="EC4" s="3">
+        <v>126</v>
+      </c>
+      <c r="ED4" s="3">
+        <v>127</v>
+      </c>
+      <c r="EE4" s="3">
+        <v>128</v>
+      </c>
+      <c r="EF4" s="3">
+        <v>129</v>
+      </c>
+      <c r="EG4" s="3">
+        <v>130</v>
+      </c>
+      <c r="EH4" s="3">
+        <v>131</v>
+      </c>
+      <c r="EI4" s="3">
+        <v>132</v>
+      </c>
+      <c r="EJ4" s="3">
+        <v>133</v>
+      </c>
+      <c r="EK4" s="3">
+        <v>134</v>
+      </c>
+      <c r="EL4" s="3">
+        <v>135</v>
+      </c>
+      <c r="EM4" s="3">
+        <v>136</v>
+      </c>
+      <c r="EN4" s="3">
+        <v>137</v>
+      </c>
+      <c r="EO4" s="3">
+        <v>138</v>
+      </c>
+      <c r="EP4" s="3">
+        <v>139</v>
+      </c>
+      <c r="EQ4" s="3">
+        <v>140</v>
+      </c>
+      <c r="ER4" s="3">
+        <v>141</v>
+      </c>
+      <c r="ES4" s="3">
+        <v>142</v>
+      </c>
+      <c r="ET4" s="3">
+        <v>143</v>
+      </c>
+      <c r="EU4" s="3">
+        <v>144</v>
+      </c>
+      <c r="EV4" s="3">
+        <v>145</v>
+      </c>
+      <c r="EW4" s="3">
+        <v>146</v>
+      </c>
+      <c r="EX4" s="3">
+        <v>147</v>
+      </c>
+      <c r="EY4" s="3">
+        <v>148</v>
+      </c>
+      <c r="EZ4" s="3">
+        <v>149</v>
+      </c>
+      <c r="FA4" s="3">
+        <v>150</v>
+      </c>
+      <c r="FB4" s="3">
+        <v>151</v>
+      </c>
+      <c r="FC4" s="3">
+        <v>152</v>
+      </c>
+      <c r="FD4" s="3">
+        <v>153</v>
+      </c>
+      <c r="FE4" s="3">
+        <v>154</v>
+      </c>
+      <c r="FF4" s="3">
+        <v>155</v>
+      </c>
+      <c r="FG4" s="3">
+        <v>156</v>
+      </c>
+      <c r="FH4" s="3">
+        <v>157</v>
+      </c>
+      <c r="FI4" s="3">
+        <v>158</v>
+      </c>
+      <c r="FJ4" s="3">
+        <v>159</v>
+      </c>
+      <c r="FK4" s="3">
+        <v>160</v>
+      </c>
+      <c r="FL4" s="3">
+        <v>161</v>
+      </c>
+      <c r="FM4" s="3">
+        <v>162</v>
+      </c>
+      <c r="FN4" s="3">
+        <v>163</v>
+      </c>
+      <c r="FO4" s="3">
+        <v>164</v>
+      </c>
+      <c r="FP4" s="3">
+        <v>165</v>
+      </c>
+      <c r="FQ4" s="3">
+        <v>166</v>
+      </c>
+      <c r="FR4" s="3">
+        <v>167</v>
+      </c>
+      <c r="FS4" s="3">
+        <v>168</v>
+      </c>
+      <c r="FT4" s="3">
+        <v>169</v>
+      </c>
+      <c r="FU4" s="3">
+        <v>170</v>
+      </c>
+      <c r="FV4" s="3">
+        <v>171</v>
+      </c>
+      <c r="FW4" s="3">
+        <v>172</v>
+      </c>
+      <c r="FX4" s="3">
+        <v>173</v>
+      </c>
+      <c r="FY4" s="3">
+        <v>174</v>
+      </c>
+      <c r="FZ4" s="3">
+        <v>175</v>
+      </c>
+      <c r="GA4" s="3">
+        <v>176</v>
+      </c>
+      <c r="GB4" s="3">
+        <v>177</v>
+      </c>
+      <c r="GC4" s="3">
+        <v>178</v>
+      </c>
+      <c r="GD4" s="3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="22">
         <v>1</v>
       </c>
-      <c r="D5" s="39">
-        <v>12</v>
-      </c>
-      <c r="E5" s="39">
+      <c r="D5" s="22">
+        <v>13</v>
+      </c>
+      <c r="E5" s="22">
         <v>1</v>
       </c>
-      <c r="F5" s="39"/>
+      <c r="F5" s="22">
+        <v>13</v>
+      </c>
       <c r="G5" s="8">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="38" t="s">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C6" s="22">
         <v>1</v>
       </c>
-      <c r="D6" s="39">
+      <c r="D6" s="22">
         <v>2</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="22">
         <v>1</v>
       </c>
-      <c r="F6" s="39">
+      <c r="F6" s="22">
         <v>6</v>
       </c>
       <c r="G6" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="38" t="s">
+    <row r="7" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="22">
         <v>2</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D7" s="22">
         <v>4</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="22">
         <v>2</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F7" s="22">
         <v>4</v>
       </c>
       <c r="G7" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="38" t="s">
+    <row r="8" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="39">
+      <c r="C8" s="22">
         <v>3</v>
       </c>
-      <c r="D8" s="39">
+      <c r="D8" s="22">
         <v>2</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="22">
         <v>3</v>
       </c>
-      <c r="F8" s="39">
+      <c r="F8" s="22">
         <v>2</v>
       </c>
       <c r="G8" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="38" t="s">
+    <row r="9" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="22">
         <v>2</v>
       </c>
-      <c r="D9" s="39">
+      <c r="D9" s="22">
         <v>1</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="22">
         <v>2</v>
       </c>
-      <c r="F9" s="39">
+      <c r="F9" s="22">
         <v>1</v>
       </c>
       <c r="G9" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="38" t="s">
+    <row r="10" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="39">
+      <c r="C10" s="22">
         <v>5</v>
       </c>
-      <c r="D10" s="39">
+      <c r="D10" s="22">
         <v>4</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="22">
         <v>6</v>
       </c>
-      <c r="F10" s="39"/>
+      <c r="F10" s="22">
+        <v>4</v>
+      </c>
       <c r="G10" s="8">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="39">
+      <c r="C11" s="22">
         <v>6</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="22">
+        <v>7</v>
+      </c>
+      <c r="E11" s="22">
         <v>6</v>
       </c>
-      <c r="E11" s="39">
-        <v>6</v>
-      </c>
-      <c r="F11" s="39"/>
+      <c r="F11" s="22">
+        <v>8</v>
+      </c>
       <c r="G11" s="8">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="38" t="s">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="39">
-        <v>13</v>
-      </c>
-      <c r="D12" s="39">
+      <c r="C12" s="22">
+        <v>14</v>
+      </c>
+      <c r="D12" s="22">
         <v>15</v>
       </c>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
       <c r="G12" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="38" t="s">
+    <row r="13" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
       <c r="G13" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="38" t="s">
+    <row r="14" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
       <c r="G14" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="38" t="s">
+    <row r="15" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="39">
+      <c r="C15" s="22">
         <v>27</v>
       </c>
-      <c r="D15" s="39">
+      <c r="D15" s="22">
         <v>21</v>
       </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
       <c r="G15" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="38" t="s">
+    <row r="16" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="39">
+      <c r="C16" s="22">
+        <v>48</v>
+      </c>
+      <c r="D16" s="22">
+        <v>52</v>
+      </c>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="22">
+        <v>100</v>
+      </c>
+      <c r="D17" s="22">
+        <v>25</v>
+      </c>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="22">
+        <v>125</v>
+      </c>
+      <c r="D18" s="22">
+        <v>5</v>
+      </c>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="22">
         <v>1</v>
       </c>
-      <c r="D16" s="39">
+      <c r="D19" s="22">
         <v>134</v>
       </c>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="8">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
+      <c r="E19" s="22">
+        <v>1</v>
+      </c>
+      <c r="F19" s="22">
+        <v>134</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0.09</v>
+      </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="6"/>
@@ -1681,7 +2082,7 @@
     <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AA2:AG2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:BO30">
+  <conditionalFormatting sqref="H5:GD30">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -1712,7 +2113,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:BO4">
+  <conditionalFormatting sqref="H4:GD4">
     <cfRule type="expression" dxfId="0" priority="8">
       <formula>H$4=period_selected</formula>
     </cfRule>

</xml_diff>

<commit_message>
Made some changes to 3 files
1. Changed usecase diagram
2. Updated project plan
3. Made changes to project plan
</commit_message>
<xml_diff>
--- a/FYP_Project_Plan.xlsx
+++ b/FYP_Project_Plan.xlsx
@@ -1042,7 +1042,7 @@
   <dimension ref="B1:GD30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="59" zoomScaleNormal="59" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="AX10" sqref="AX10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1078,7 +1078,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="14">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J2" s="15"/>
       <c r="K2" s="32" t="s">
@@ -1719,16 +1719,16 @@
         <v>1</v>
       </c>
       <c r="D5" s="22">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E5" s="22">
         <v>1</v>
       </c>
       <c r="F5" s="22">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G5" s="8">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="6" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
small changes to project plan
</commit_message>
<xml_diff>
--- a/FYP_Project_Plan.xlsx
+++ b/FYP_Project_Plan.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>PERIODS</t>
   </si>
@@ -177,9 +177,6 @@
   </si>
   <si>
     <t>FYP Project Planner</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Inception 1: Listing possible risk that may occure</t>
@@ -1042,7 +1039,7 @@
   <dimension ref="B1:GD30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="59" zoomScaleNormal="59" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AX10" sqref="AX10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1813,7 +1810,7 @@
     </row>
     <row r="10" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="22">
         <v>5</v>
@@ -1871,8 +1868,8 @@
       <c r="B13" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="22" t="s">
-        <v>23</v>
+      <c r="C13" s="22">
+        <v>9</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -1883,10 +1880,10 @@
     </row>
     <row r="14" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="C14" s="22">
+        <v>9</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -1897,7 +1894,7 @@
     </row>
     <row r="15" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="22">
         <v>27</v>
@@ -1913,7 +1910,7 @@
     </row>
     <row r="16" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="22">
         <v>48</v>
@@ -1929,7 +1926,7 @@
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="22">
         <v>100</v>
@@ -1945,7 +1942,7 @@
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="22">
         <v>125</v>
@@ -1961,7 +1958,7 @@
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="22">
         <v>1</v>

</xml_diff>